<commit_message>
buffer grilla zona incendios
</commit_message>
<xml_diff>
--- a/info_papers.xlsx
+++ b/info_papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\magister\propagacion-incendios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A0B872-3151-4EFC-89C6-C8BC90A85EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF765509-0072-4C77-A057-906390B7C077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{66D5AC22-24BE-4795-8951-5D4A0EEF5911}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Paper</t>
   </si>
@@ -208,9 +208,6 @@
     <t>Spatial variability in Arctic–boreal fire regimes influenced by environmental and human factors</t>
   </si>
   <si>
-    <t>Baja importancia</t>
-  </si>
-  <si>
     <t>paquete Mclust: modelo de cluster mezcla gaussiana finita</t>
   </si>
   <si>
@@ -229,9 +226,6 @@
     <t>Next Day Wildfire Spread: A Machine Learning Dataset to Predict Wildfire Spreading From Remote-Sensing Data</t>
   </si>
   <si>
-    <t>Le va pésimo</t>
-  </si>
-  <si>
     <t>https://journals.ametsoc.org/view/journals/aies/3/3/AIES-D-23-0087.1.xml</t>
   </si>
   <si>
@@ -269,6 +263,16 @@
   </si>
   <si>
     <t>Fire Intensity and spRead forecAst (FIRA): A Machine Learning Based Fire Spread Prediction Model for Air Quality Forecasting Application</t>
+  </si>
+  <si>
+    <t>Según los puntos donde sabemos que se quemó algo en un día dado, estimamos por interpolación cuándo (qué día) se quemaron las demás celdas"</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2503.08580</t>
+  </si>
+  <si>
+    <t>Comparing Next-Day Wildfire Predictability of
+MODIS and VIIRS Satellite Data</t>
   </si>
 </sst>
 </file>
@@ -737,25 +741,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAFF9BD-90D0-405C-A75D-86DB60E838DA}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="22.85546875" customWidth="1"/>
+    <col min="8" max="9" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -784,7 +788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
@@ -810,7 +814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -829,8 +833,11 @@
       <c r="I3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>31</v>
       </c>
@@ -847,82 +854,85 @@
         <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="9" t="s">
+    </row>
+    <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>26</v>
       </c>
@@ -940,9 +950,10 @@
     <hyperlink ref="B8" r:id="rId9" xr:uid="{3C41ECD5-4B6F-4023-A445-BEA7B1202B65}"/>
     <hyperlink ref="B10" r:id="rId10" xr:uid="{BAFFED2F-59DE-44CE-9896-544B71E6E2D4}"/>
     <hyperlink ref="B9" r:id="rId11" xr:uid="{9221BA70-A21C-44C9-9B92-F08C8B4A568A}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{7FBDFC1B-D332-453A-B6B5-723F388C7AA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -954,24 +965,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -987,9 +998,9 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>

</xml_diff>